<commit_message>
new netball r file and african football legends data
</commit_message>
<xml_diff>
--- a/sub_pro_9_fb_ref_big_5_euro_league/datasets/african_football_legends.xlsx
+++ b/sub_pro_9_fb_ref_big_5_euro_league/datasets/african_football_legends.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R_Files\sports_data_sci\sub_pro_9_fb_ref_big_5_euro_league\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66CB79BA-1A9B-4C4A-9353-4A2E82C2E62D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D819DE7C-3319-49E9-8624-A4D87401C208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="349" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="177">
   <si>
     <t>Player</t>
   </si>
@@ -407,6 +407,150 @@
   </si>
   <si>
     <t>Juventus</t>
+  </si>
+  <si>
+    <t>03_04</t>
+  </si>
+  <si>
+    <t>Inter</t>
+  </si>
+  <si>
+    <t>Obafemi Martins</t>
+  </si>
+  <si>
+    <t>Yakubu Aiyegbeni</t>
+  </si>
+  <si>
+    <t>Everton</t>
+  </si>
+  <si>
+    <t>Kelechi Iheanacho</t>
+  </si>
+  <si>
+    <t>Ademola Lookman</t>
+  </si>
+  <si>
+    <t>RB Leipzig</t>
+  </si>
+  <si>
+    <t>Dortmund</t>
+  </si>
+  <si>
+    <t>22_23</t>
+  </si>
+  <si>
+    <t>Sébastien Haller</t>
+  </si>
+  <si>
+    <t>Inaki Williams</t>
+  </si>
+  <si>
+    <t>15_16</t>
+  </si>
+  <si>
+    <t>Athletic Club</t>
+  </si>
+  <si>
+    <t>Paul Onuachu</t>
+  </si>
+  <si>
+    <t>Andy Delort</t>
+  </si>
+  <si>
+    <t>Simon Adingra</t>
+  </si>
+  <si>
+    <t>Alex Iwobi</t>
+  </si>
+  <si>
+    <t>Wilfrid Zaha</t>
+  </si>
+  <si>
+    <t>Habib Diallo</t>
+  </si>
+  <si>
+    <t>Sofiane Boufal</t>
+  </si>
+  <si>
+    <t>Patson Daka</t>
+  </si>
+  <si>
+    <t>Umar Sadiq</t>
+  </si>
+  <si>
+    <t>Taiwo Awoniyi</t>
+  </si>
+  <si>
+    <t>Musa Barrow</t>
+  </si>
+  <si>
+    <t>Ihlas Bebou</t>
+  </si>
+  <si>
+    <t>Southampton</t>
+  </si>
+  <si>
+    <t>24_25</t>
+  </si>
+  <si>
+    <t>20_21</t>
+  </si>
+  <si>
+    <t>Montpellier</t>
+  </si>
+  <si>
+    <t>Youssef En-Nesyri</t>
+  </si>
+  <si>
+    <t>Boulaye Dia</t>
+  </si>
+  <si>
+    <t>Salernitana</t>
+  </si>
+  <si>
+    <t>Defender / Forward / Midfielder</t>
+  </si>
+  <si>
+    <t>Brighton</t>
+  </si>
+  <si>
+    <t>Crystal Palace</t>
+  </si>
+  <si>
+    <t>Strasbourg</t>
+  </si>
+  <si>
+    <t>14_15</t>
+  </si>
+  <si>
+    <t>Lille</t>
+  </si>
+  <si>
+    <t>Leicester City</t>
+  </si>
+  <si>
+    <t>Valencia</t>
+  </si>
+  <si>
+    <t>Nottingham Forest</t>
+  </si>
+  <si>
+    <t>Gambia</t>
+  </si>
+  <si>
+    <t>Atalanta</t>
+  </si>
+  <si>
+    <t>Odion Ighalo</t>
+  </si>
+  <si>
+    <t>Watford</t>
+  </si>
+  <si>
+    <t>Hoffenheim</t>
+  </si>
+  <si>
+    <t>Amad Diallo</t>
   </si>
 </sst>
 </file>
@@ -788,17 +932,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C17636A1-2981-4DB0-A9BA-531E3106FEDD}">
-  <dimension ref="A1:L42"/>
+  <dimension ref="A1:L64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64:L64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.54296875" customWidth="1"/>
+    <col min="4" max="4" width="28.08984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.6328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.36328125" customWidth="1"/>
     <col min="7" max="7" width="26.7265625" bestFit="1" customWidth="1"/>
@@ -2396,6 +2540,842 @@
         <v>0.73</v>
       </c>
     </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" t="s">
+        <v>60</v>
+      </c>
+      <c r="E43">
+        <v>14.3</v>
+      </c>
+      <c r="F43" t="s">
+        <v>129</v>
+      </c>
+      <c r="G43" t="s">
+        <v>130</v>
+      </c>
+      <c r="H43">
+        <v>0.49</v>
+      </c>
+      <c r="I43">
+        <v>0.42</v>
+      </c>
+      <c r="J43">
+        <v>0.91</v>
+      </c>
+      <c r="K43">
+        <v>0.49</v>
+      </c>
+      <c r="L43">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>132</v>
+      </c>
+      <c r="B44" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" t="s">
+        <v>60</v>
+      </c>
+      <c r="E44">
+        <v>12.2</v>
+      </c>
+      <c r="F44" t="s">
+        <v>73</v>
+      </c>
+      <c r="G44" t="s">
+        <v>133</v>
+      </c>
+      <c r="H44">
+        <v>0.41</v>
+      </c>
+      <c r="I44">
+        <v>0.33</v>
+      </c>
+      <c r="J44">
+        <v>0.74</v>
+      </c>
+      <c r="K44">
+        <v>0.41</v>
+      </c>
+      <c r="L44">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>134</v>
+      </c>
+      <c r="B45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" t="s">
+        <v>113</v>
+      </c>
+      <c r="E45">
+        <v>6</v>
+      </c>
+      <c r="F45" t="s">
+        <v>86</v>
+      </c>
+      <c r="G45" t="s">
+        <v>96</v>
+      </c>
+      <c r="H45">
+        <v>0.67</v>
+      </c>
+      <c r="I45">
+        <v>0.5</v>
+      </c>
+      <c r="J45">
+        <v>1.17</v>
+      </c>
+      <c r="K45">
+        <v>0.67</v>
+      </c>
+      <c r="L45">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>135</v>
+      </c>
+      <c r="B46" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" t="s">
+        <v>55</v>
+      </c>
+      <c r="D46" t="s">
+        <v>113</v>
+      </c>
+      <c r="E46">
+        <v>6.4</v>
+      </c>
+      <c r="F46" t="s">
+        <v>93</v>
+      </c>
+      <c r="G46" t="s">
+        <v>136</v>
+      </c>
+      <c r="H46">
+        <v>0.78</v>
+      </c>
+      <c r="I46">
+        <v>0.47</v>
+      </c>
+      <c r="J46">
+        <v>1.25</v>
+      </c>
+      <c r="K46">
+        <v>0.78</v>
+      </c>
+      <c r="L46">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>139</v>
+      </c>
+      <c r="B47" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" t="s">
+        <v>60</v>
+      </c>
+      <c r="E47">
+        <v>13.6</v>
+      </c>
+      <c r="F47" t="s">
+        <v>138</v>
+      </c>
+      <c r="G47" t="s">
+        <v>137</v>
+      </c>
+      <c r="H47">
+        <v>0.66</v>
+      </c>
+      <c r="I47">
+        <v>0.22</v>
+      </c>
+      <c r="J47">
+        <v>0.88</v>
+      </c>
+      <c r="K47">
+        <v>0.66</v>
+      </c>
+      <c r="L47">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>140</v>
+      </c>
+      <c r="B48" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" t="s">
+        <v>55</v>
+      </c>
+      <c r="D48" t="s">
+        <v>113</v>
+      </c>
+      <c r="E48">
+        <v>18</v>
+      </c>
+      <c r="F48" t="s">
+        <v>141</v>
+      </c>
+      <c r="G48" t="s">
+        <v>142</v>
+      </c>
+      <c r="H48">
+        <v>0.44</v>
+      </c>
+      <c r="I48">
+        <v>0.17</v>
+      </c>
+      <c r="J48">
+        <v>0.61</v>
+      </c>
+      <c r="K48">
+        <v>0.44</v>
+      </c>
+      <c r="L48">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>143</v>
+      </c>
+      <c r="B49" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" t="s">
+        <v>55</v>
+      </c>
+      <c r="D49" t="s">
+        <v>60</v>
+      </c>
+      <c r="E49">
+        <v>11.7</v>
+      </c>
+      <c r="F49" t="s">
+        <v>156</v>
+      </c>
+      <c r="G49" t="s">
+        <v>155</v>
+      </c>
+      <c r="H49">
+        <v>0.34</v>
+      </c>
+      <c r="I49">
+        <v>0.09</v>
+      </c>
+      <c r="J49">
+        <v>0.43</v>
+      </c>
+      <c r="K49">
+        <v>0.34</v>
+      </c>
+      <c r="L49">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>144</v>
+      </c>
+      <c r="B50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" t="s">
+        <v>56</v>
+      </c>
+      <c r="D50" t="s">
+        <v>60</v>
+      </c>
+      <c r="E50">
+        <v>27.6</v>
+      </c>
+      <c r="F50" t="s">
+        <v>157</v>
+      </c>
+      <c r="G50" t="s">
+        <v>158</v>
+      </c>
+      <c r="H50">
+        <v>0.54</v>
+      </c>
+      <c r="I50">
+        <v>0.33</v>
+      </c>
+      <c r="J50">
+        <v>0.87</v>
+      </c>
+      <c r="K50">
+        <v>0.54</v>
+      </c>
+      <c r="L50">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>159</v>
+      </c>
+      <c r="B51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51" t="s">
+        <v>56</v>
+      </c>
+      <c r="D51" t="s">
+        <v>60</v>
+      </c>
+      <c r="E51">
+        <v>25.7</v>
+      </c>
+      <c r="F51" t="s">
+        <v>157</v>
+      </c>
+      <c r="G51" t="s">
+        <v>90</v>
+      </c>
+      <c r="H51">
+        <v>0.7</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>0.7</v>
+      </c>
+      <c r="K51">
+        <v>0.7</v>
+      </c>
+      <c r="L51">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>160</v>
+      </c>
+      <c r="B52" t="s">
+        <v>39</v>
+      </c>
+      <c r="C52" t="s">
+        <v>55</v>
+      </c>
+      <c r="D52" t="s">
+        <v>113</v>
+      </c>
+      <c r="E52">
+        <v>28</v>
+      </c>
+      <c r="F52" t="s">
+        <v>138</v>
+      </c>
+      <c r="G52" t="s">
+        <v>161</v>
+      </c>
+      <c r="H52">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="I52">
+        <v>0.21</v>
+      </c>
+      <c r="J52">
+        <v>0.79</v>
+      </c>
+      <c r="K52">
+        <v>0.54</v>
+      </c>
+      <c r="L52">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>145</v>
+      </c>
+      <c r="B53" t="s">
+        <v>38</v>
+      </c>
+      <c r="C53" t="s">
+        <v>55</v>
+      </c>
+      <c r="D53" t="s">
+        <v>162</v>
+      </c>
+      <c r="E53">
+        <v>12.2</v>
+      </c>
+      <c r="F53" t="s">
+        <v>156</v>
+      </c>
+      <c r="G53" t="s">
+        <v>163</v>
+      </c>
+      <c r="H53">
+        <v>0.16</v>
+      </c>
+      <c r="I53">
+        <v>0.16</v>
+      </c>
+      <c r="J53">
+        <v>0.33</v>
+      </c>
+      <c r="K53">
+        <v>0.16</v>
+      </c>
+      <c r="L53">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>146</v>
+      </c>
+      <c r="B54" t="s">
+        <v>40</v>
+      </c>
+      <c r="C54" t="s">
+        <v>55</v>
+      </c>
+      <c r="D54" t="s">
+        <v>113</v>
+      </c>
+      <c r="E54">
+        <v>7</v>
+      </c>
+      <c r="F54" t="s">
+        <v>141</v>
+      </c>
+      <c r="G54" t="s">
+        <v>71</v>
+      </c>
+      <c r="H54">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="I54">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="J54">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="K54">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="L54">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>147</v>
+      </c>
+      <c r="B55" t="s">
+        <v>38</v>
+      </c>
+      <c r="C55" t="s">
+        <v>55</v>
+      </c>
+      <c r="D55" t="s">
+        <v>113</v>
+      </c>
+      <c r="E55">
+        <v>33.5</v>
+      </c>
+      <c r="F55" t="s">
+        <v>86</v>
+      </c>
+      <c r="G55" t="s">
+        <v>164</v>
+      </c>
+      <c r="H55">
+        <v>0.21</v>
+      </c>
+      <c r="I55">
+        <v>0.24</v>
+      </c>
+      <c r="J55">
+        <v>0.45</v>
+      </c>
+      <c r="K55">
+        <v>0.21</v>
+      </c>
+      <c r="L55">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>148</v>
+      </c>
+      <c r="B56" t="s">
+        <v>39</v>
+      </c>
+      <c r="C56" t="s">
+        <v>55</v>
+      </c>
+      <c r="D56" t="s">
+        <v>60</v>
+      </c>
+      <c r="E56">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="F56" t="s">
+        <v>97</v>
+      </c>
+      <c r="G56" t="s">
+        <v>165</v>
+      </c>
+      <c r="H56">
+        <v>0.64</v>
+      </c>
+      <c r="I56">
+        <v>0.06</v>
+      </c>
+      <c r="J56">
+        <v>0.7</v>
+      </c>
+      <c r="K56">
+        <v>0.53</v>
+      </c>
+      <c r="L56">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>149</v>
+      </c>
+      <c r="B57" t="s">
+        <v>49</v>
+      </c>
+      <c r="C57" t="s">
+        <v>56</v>
+      </c>
+      <c r="D57" t="s">
+        <v>113</v>
+      </c>
+      <c r="E57">
+        <v>11.3</v>
+      </c>
+      <c r="F57" t="s">
+        <v>166</v>
+      </c>
+      <c r="G57" t="s">
+        <v>167</v>
+      </c>
+      <c r="H57">
+        <v>0.27</v>
+      </c>
+      <c r="I57">
+        <v>0.53</v>
+      </c>
+      <c r="J57">
+        <v>0.8</v>
+      </c>
+      <c r="K57">
+        <v>0.09</v>
+      </c>
+      <c r="L57">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>150</v>
+      </c>
+      <c r="B58" t="s">
+        <v>54</v>
+      </c>
+      <c r="C58" t="s">
+        <v>59</v>
+      </c>
+      <c r="D58" t="s">
+        <v>60</v>
+      </c>
+      <c r="E58">
+        <v>12.9</v>
+      </c>
+      <c r="F58" t="s">
+        <v>97</v>
+      </c>
+      <c r="G58" t="s">
+        <v>168</v>
+      </c>
+      <c r="H58">
+        <v>0.39</v>
+      </c>
+      <c r="I58">
+        <v>0.23</v>
+      </c>
+      <c r="J58">
+        <v>0.62</v>
+      </c>
+      <c r="K58">
+        <v>0.39</v>
+      </c>
+      <c r="L58">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>151</v>
+      </c>
+      <c r="B59" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59" t="s">
+        <v>55</v>
+      </c>
+      <c r="D59" t="s">
+        <v>60</v>
+      </c>
+      <c r="E59">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="F59" t="s">
+        <v>156</v>
+      </c>
+      <c r="G59" t="s">
+        <v>169</v>
+      </c>
+      <c r="H59">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K59">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L59">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>152</v>
+      </c>
+      <c r="B60" t="s">
+        <v>40</v>
+      </c>
+      <c r="C60" t="s">
+        <v>55</v>
+      </c>
+      <c r="D60" t="s">
+        <v>60</v>
+      </c>
+      <c r="E60">
+        <v>11.6</v>
+      </c>
+      <c r="F60" t="s">
+        <v>119</v>
+      </c>
+      <c r="G60" t="s">
+        <v>170</v>
+      </c>
+      <c r="H60">
+        <v>0.52</v>
+      </c>
+      <c r="I60">
+        <v>0.26</v>
+      </c>
+      <c r="J60">
+        <v>0.78</v>
+      </c>
+      <c r="K60">
+        <v>0.52</v>
+      </c>
+      <c r="L60">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>153</v>
+      </c>
+      <c r="B61" t="s">
+        <v>171</v>
+      </c>
+      <c r="C61" t="s">
+        <v>55</v>
+      </c>
+      <c r="D61" t="s">
+        <v>113</v>
+      </c>
+      <c r="E61">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F61" t="s">
+        <v>93</v>
+      </c>
+      <c r="G61" t="s">
+        <v>172</v>
+      </c>
+      <c r="H61">
+        <v>0.61</v>
+      </c>
+      <c r="I61">
+        <v>0.2</v>
+      </c>
+      <c r="J61">
+        <v>0.81</v>
+      </c>
+      <c r="K61">
+        <v>0.61</v>
+      </c>
+      <c r="L61">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>173</v>
+      </c>
+      <c r="B62" t="s">
+        <v>40</v>
+      </c>
+      <c r="C62" t="s">
+        <v>55</v>
+      </c>
+      <c r="D62" t="s">
+        <v>60</v>
+      </c>
+      <c r="E62">
+        <v>35</v>
+      </c>
+      <c r="F62" t="s">
+        <v>141</v>
+      </c>
+      <c r="G62" t="s">
+        <v>174</v>
+      </c>
+      <c r="H62">
+        <v>0.43</v>
+      </c>
+      <c r="I62">
+        <v>0.09</v>
+      </c>
+      <c r="J62">
+        <v>0.51</v>
+      </c>
+      <c r="K62">
+        <v>0.43</v>
+      </c>
+      <c r="L62">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>154</v>
+      </c>
+      <c r="B63" t="s">
+        <v>42</v>
+      </c>
+      <c r="C63" t="s">
+        <v>55</v>
+      </c>
+      <c r="D63" t="s">
+        <v>113</v>
+      </c>
+      <c r="E63">
+        <v>18.2</v>
+      </c>
+      <c r="F63" t="s">
+        <v>119</v>
+      </c>
+      <c r="G63" t="s">
+        <v>175</v>
+      </c>
+      <c r="H63">
+        <v>0.39</v>
+      </c>
+      <c r="I63">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="J63">
+        <v>0.66</v>
+      </c>
+      <c r="K63">
+        <v>0.39</v>
+      </c>
+      <c r="L63">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>176</v>
+      </c>
+      <c r="B64" t="s">
+        <v>38</v>
+      </c>
+      <c r="C64" t="s">
+        <v>55</v>
+      </c>
+      <c r="D64" t="s">
+        <v>113</v>
+      </c>
+      <c r="E64">
+        <v>21.1</v>
+      </c>
+      <c r="F64" t="s">
+        <v>156</v>
+      </c>
+      <c r="G64" t="s">
+        <v>122</v>
+      </c>
+      <c r="H64">
+        <v>0.38</v>
+      </c>
+      <c r="I64">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="J64">
+        <v>0.66</v>
+      </c>
+      <c r="K64">
+        <v>0.38</v>
+      </c>
+      <c r="L64">
+        <v>0.66</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L55">
     <sortCondition ref="D1:D55"/>

</xml_diff>